<commit_message>
update elara types and add sequencer apps docs
</commit_message>
<xml_diff>
--- a/doc/elara-app-types.xlsx
+++ b/doc/elara-app-types.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>Elara Application Types (Overview)</t>
   </si>
@@ -37,7 +37,7 @@
 Distribution</t>
   </si>
   <si>
-    <t>SubscriberApp</t>
+    <t>InputApp</t>
   </si>
   <si>
     <t>y</t>
@@ -52,7 +52,7 @@
     <t>ProcessorApp</t>
   </si>
   <si>
-    <t>PublisherApp</t>
+    <t>OutputApp</t>
   </si>
   <si>
     <t>TimerApp</t>
@@ -70,7 +70,7 @@
     <t>PlaybackApp</t>
   </si>
   <si>
-    <t>ReplicatorApp</t>
+    <t>ReplicationApp</t>
   </si>
   <si>
     <t>(p)</t>
@@ -127,13 +127,46 @@
     <t>Typically non-deterministic since source of messages is usually not deterministic</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Uses </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Command Sender </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>to send input message to the sequencer as a command</t>
+    </r>
+  </si>
+  <si>
+    <t>Command Sending</t>
+  </si>
+  <si>
+    <t>Assigns source ID and sequence to a message and sends the message — now called command — to the sequencer</t>
+  </si>
+  <si>
+    <t>Commands can originate from different situations, but mostly from inputs or in reaction to events</t>
+  </si>
+  <si>
     <t>Command Sequencing</t>
   </si>
   <si>
-    <t>Sequences multiple inputs into a defined sequence of commands</t>
-  </si>
-  <si>
-    <t>Converts input message to a command and hereby assigns source ID, source sequence and timestamp to each command</t>
+    <t>Sequences commands from multiple streams into a defined sequence of commands</t>
   </si>
   <si>
     <t>Non-deterministic since multiple input sources are connected and racing can occur between the sources</t>
@@ -145,7 +178,16 @@
     <t>Has read-only access to application state</t>
   </si>
   <si>
-    <t>Event Application</t>
+    <t>Event Routing</t>
+  </si>
+  <si>
+    <t>Process of creating an event in the command processor</t>
+  </si>
+  <si>
+    <t>When the event is complete it is routed, which means it is stored in the event store and typically also immediately applied to the processor’s application state, and later possibly also picked for output distribution</t>
+  </si>
+  <si>
+    <t>Event Applying</t>
   </si>
   <si>
     <t>Modification of application state by applying events</t>
@@ -181,10 +223,57 @@
     <t>Adapts transport and codec from source system to sequencer app</t>
   </si>
   <si>
+    <t>Assigns source ID and source sequence and sends commands to sequencer</t>
+  </si>
+  <si>
     <t>Multiple active subscriber apps can be present in a running Elara multi-application installation</t>
   </si>
   <si>
-    <t>Can optionally also perform input adaptation and codec transformation if this is not done in an upstream subscriber app already</t>
+    <t>Sequences multiple command streams into a single sequenced stream</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Sequenced commands are either (i) stored in a command store and later polled and processed via </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>PollerProcessorApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">, or (ii) directly processed (see </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>SequencerProcessorApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
   <si>
     <t>Only one sequencer app is active at any point in time in a running Elara multi-application installation</t>
@@ -199,9 +288,86 @@
     <t>Has read/write access to application state while applying a routed event to the application state</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">App type exists in two variants: </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>PollerProcessorApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>SequencerProcessorApp</t>
+    </r>
+  </si>
+  <si>
     <t>Only one processor app is active at any point in time in a running Elara multi-application installation</t>
   </si>
   <si>
+    <t>PollerProcessorApp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>ProcessorApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> that polls commands to process from a command store</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>SequencerApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> that directly invokes command processor with sequenced commands; no command store is present</t>
+    </r>
+  </si>
+  <si>
     <t>Publishes messages to downstream applications based on events</t>
   </si>
   <si>
@@ -256,15 +422,15 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>SequencerApp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
+      <t xml:space="preserve">SequencerApp, ProcessorApp </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
     </r>
     <r>
       <rPr>
@@ -273,25 +439,28 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>ProcessorApp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> where both functions are processed in a single-threaded Application</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">Combination of </t>
+      <t>PublisherApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> n a single-threaded Application</t>
+    </r>
+  </si>
+  <si>
+    <t>Performs all functions from input adaptation and sequencing to command processing and output publishing and hence can act as a fully featured application</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Since output publishing is processed in the same thread as sequencing, this application type supports a direct command loopback feature which allows insertion of commands directly into the front of the command queue when processing output events.  This can be seen as a special case of an embedded </t>
     </r>
     <r>
       <rPr>
@@ -300,15 +469,37 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve">SequencerApp, ProcessorApp </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">and </t>
+      <t>FeedbackApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> where commands are sent back to the sequencer (but not added to the front of the queue in this case)</t>
+    </r>
+  </si>
+  <si>
+    <t>A fully-deterministic application that consumes events, updates the application state and outputs commands</t>
+  </si>
+  <si>
+    <t>This type of application allows parallelisation of functionality and remove computing load from the ProcessorApp</t>
+  </si>
+  <si>
+    <t>Multiple active feedback apps can be present in a running Elara multi-application installation</t>
+  </si>
+  <si>
+    <t>A special application for publishing events on request by subscribing apps</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">An example client is the </t>
     </r>
     <r>
       <rPr>
@@ -317,28 +508,28 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>PublisherApp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> n a single-threaded Application</t>
-    </r>
-  </si>
-  <si>
-    <t>Performs all functions from input adaptation and sequencing to command processing and output publishing and hence can act as a fully featured application</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">Since output publishing is processed in the same thread as sequencing, this application type supports a direct command loopback feature which allows insertion of commands directly into the front of the command queue when processing output events.  This can be seen as a special case of an embedded </t>
+      <t>ReplicationApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> but playback app can also be used to bring restarted nodes back in sync</t>
+    </r>
+  </si>
+  <si>
+    <t>Multiple active playback apps can be present in a running Elara multi-application installation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Subscribes for event playback using the </t>
     </r>
     <r>
       <rPr>
@@ -347,75 +538,6 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>FeedbackApp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> where commands are also generated on the back of an event stream.</t>
-    </r>
-  </si>
-  <si>
-    <t>A fully-deterministic application that consumes events, updates the application state and outputs commands</t>
-  </si>
-  <si>
-    <t>This type of application allows parallelisation of functionality and remove computing load from the ProcessorApp</t>
-  </si>
-  <si>
-    <t>Multiple active feedback apps can be present in a running Elara multi-application installation</t>
-  </si>
-  <si>
-    <t>A special application for publishing events on request by subscribing apps</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">An example client is the </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="1"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>ReplicatorApp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> but playback app can also be used to bring restarted nodes back in sync</t>
-    </r>
-  </si>
-  <si>
-    <t>Multiple active playback apps can be present in a running Elara multi-application installation</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">Subscribes for event playback using the </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="1"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
       <t>PlaybackApp</t>
     </r>
     <r>
@@ -424,11 +546,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve"> and reproduces an exact copy of the event log on another host</t>
-    </r>
-  </si>
-  <si>
-    <t>Event log copies can be created for cold or warm standby applications, or purely for backup purposes for test regression replays</t>
+      <t xml:space="preserve"> and reproduces an exact copy of the event store on another host</t>
+    </r>
+  </si>
+  <si>
+    <t>Event store copies can be created for cold or warm standby applications, or purely for backup purposes for test regression replays</t>
   </si>
   <si>
     <t>Multiple active replication apps can be present in a running Elara multi-application installation</t>
@@ -630,7 +752,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -656,13 +778,7 @@
     <font>
       <i val="1"/>
       <sz val="10"/>
-      <color indexed="16"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <i val="1"/>
-      <sz val="10"/>
-      <color indexed="17"/>
+      <color indexed="15"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -711,15 +827,15 @@
     <fill>
       <gradientFill type="linear" degree="0">
         <stop position="0">
-          <color rgb="fffefdd5"/>
+          <color rgb="4dfefb00"/>
         </stop>
         <stop position="1">
-          <color rgb="ffd4feff"/>
+          <color rgb="4b0096ff"/>
         </stop>
       </gradientFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -772,73 +888,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -875,49 +931,46 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -943,11 +996,9 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="fffefdd5"/>
-      <rgbColor rgb="ffd4feff"/>
+      <rgbColor rgb="fffefdb3"/>
+      <rgbColor rgb="ffb1dfff"/>
       <rgbColor rgb="ffa9a9a9"/>
-      <rgbColor rgb="ffd0d0d0"/>
-      <rgbColor rgb="ff797979"/>
       <rgbColor rgb="ff929292"/>
     </indexedColors>
   </colors>
@@ -3820,7 +3871,7 @@
       <c r="A18" t="s" s="13">
         <v>21</v>
       </c>
-      <c r="B18" s="14"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -3828,10 +3879,10 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="15">
+      <c r="A19" t="s" s="14">
         <v>22</v>
       </c>
-      <c r="B19" s="14"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -3839,10 +3890,10 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="16">
+      <c r="A20" t="s" s="15">
         <v>23</v>
       </c>
-      <c r="B20" s="14"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -3861,7 +3912,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="18">
+      <c r="A22" t="s" s="17">
         <v>25</v>
       </c>
       <c r="B22" s="7"/>
@@ -3872,7 +3923,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="19">
+      <c r="A23" t="s" s="18">
         <v>26</v>
       </c>
       <c r="B23" s="7"/>
@@ -3883,7 +3934,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="19">
+      <c r="A24" t="s" s="18">
         <v>27</v>
       </c>
       <c r="B24" s="7"/>
@@ -3894,7 +3945,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="19">
+      <c r="A25" t="s" s="18">
         <v>28</v>
       </c>
       <c r="B25" s="7"/>
@@ -3923,11 +3974,8 @@
       <c r="G27" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="C5"/>
-    <mergeCell ref="A5"/>
-    <mergeCell ref="B5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3943,16 +3991,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:C22"/>
+  <dimension ref="A2:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.08594" style="20" customWidth="1"/>
-    <col min="2" max="2" width="2.54688" style="20" customWidth="1"/>
-    <col min="3" max="3" width="99.25" style="20" customWidth="1"/>
-    <col min="4" max="16384" width="16.3516" style="20" customWidth="1"/>
+    <col min="1" max="1" width="5.08594" style="19" customWidth="1"/>
+    <col min="2" max="2" width="2.54688" style="19" customWidth="1"/>
+    <col min="3" max="4" width="99.25" style="19" customWidth="1"/>
+    <col min="5" max="16384" width="16.3516" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -3961,189 +4009,267 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" ht="23" customHeight="1">
-      <c r="A2" t="s" s="21">
+      <c r="A2" t="s" s="20">
         <v>30</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" ht="23" customHeight="1">
-      <c r="A3" s="24"/>
-      <c r="B3" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s" s="26">
+      <c r="A3" s="23"/>
+      <c r="B3" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s" s="25">
         <v>32</v>
       </c>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" ht="23" customHeight="1">
-      <c r="A4" s="24"/>
-      <c r="B4" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s" s="26">
+      <c r="A4" s="23"/>
+      <c r="B4" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s" s="25">
         <v>33</v>
       </c>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" ht="23" customHeight="1">
-      <c r="A5" s="24"/>
-      <c r="B5" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s" s="26">
+      <c r="A5" s="23"/>
+      <c r="B5" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s" s="25">
         <v>34</v>
       </c>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" ht="23" customHeight="1">
-      <c r="A6" s="24"/>
-      <c r="B6" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s" s="26">
+      <c r="A6" s="23"/>
+      <c r="B6" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s" s="25">
         <v>35</v>
       </c>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" ht="23" customHeight="1">
-      <c r="A7" t="s" s="21">
+      <c r="A7" s="23"/>
+      <c r="B7" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s" s="25">
         <v>36</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="8" ht="23" customHeight="1">
-      <c r="A8" s="24"/>
-      <c r="B8" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s" s="26">
+      <c r="A8" t="s" s="20">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" ht="32" customHeight="1">
-      <c r="A9" s="24"/>
-      <c r="B9" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s" s="26">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" ht="23" customHeight="1">
+      <c r="A9" s="23"/>
+      <c r="B9" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s" s="25">
         <v>38</v>
       </c>
+      <c r="D9" s="22"/>
     </row>
     <row r="10" ht="23" customHeight="1">
-      <c r="A10" s="24"/>
-      <c r="B10" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s" s="26">
+      <c r="A10" s="23"/>
+      <c r="B10" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s" s="25">
         <v>39</v>
       </c>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" ht="23" customHeight="1">
-      <c r="A11" t="s" s="21">
+      <c r="A11" t="s" s="20">
+        <v>40</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" ht="23" customHeight="1">
+      <c r="A12" s="23"/>
+      <c r="B12" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s" s="25">
+        <v>41</v>
+      </c>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" ht="23" customHeight="1">
+      <c r="A13" s="23"/>
+      <c r="B13" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s" s="25">
+        <v>42</v>
+      </c>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" ht="23" customHeight="1">
+      <c r="A14" t="s" s="20">
         <v>3</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-    </row>
-    <row r="12" ht="23" customHeight="1">
-      <c r="A12" s="24"/>
-      <c r="B12" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s" s="26">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" ht="23" customHeight="1">
-      <c r="A13" s="24"/>
-      <c r="B13" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s" s="26">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" ht="23" customHeight="1">
-      <c r="A14" t="s" s="21">
-        <v>42</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
     </row>
     <row r="15" ht="23" customHeight="1">
-      <c r="A15" s="24"/>
-      <c r="B15" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s" s="26">
+      <c r="A15" s="23"/>
+      <c r="B15" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s" s="25">
         <v>43</v>
       </c>
+      <c r="D15" s="22"/>
     </row>
     <row r="16" ht="23" customHeight="1">
-      <c r="A16" s="24"/>
-      <c r="B16" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s" s="26">
+      <c r="A16" s="23"/>
+      <c r="B16" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s" s="25">
         <v>44</v>
       </c>
+      <c r="D16" s="22"/>
     </row>
     <row r="17" ht="23" customHeight="1">
-      <c r="A17" s="24"/>
-      <c r="B17" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s" s="26">
+      <c r="A17" t="s" s="20">
         <v>45</v>
       </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
     </row>
     <row r="18" ht="23" customHeight="1">
-      <c r="A18" t="s" s="21">
+      <c r="A18" s="23"/>
+      <c r="B18" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s" s="25">
         <v>46</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-    </row>
-    <row r="19" ht="23" customHeight="1">
-      <c r="A19" s="24"/>
-      <c r="B19" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s" s="26">
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" ht="32" customHeight="1">
+      <c r="A19" s="23"/>
+      <c r="B19" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s" s="25">
         <v>47</v>
       </c>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" ht="23" customHeight="1">
-      <c r="A20" s="24"/>
-      <c r="B20" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C20" t="s" s="26">
+      <c r="A20" t="s" s="20">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" ht="32" customHeight="1">
-      <c r="A21" s="24"/>
-      <c r="B21" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C21" t="s" s="26">
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" ht="23" customHeight="1">
+      <c r="A21" s="23"/>
+      <c r="B21" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s" s="25">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" ht="32" customHeight="1">
-      <c r="A22" s="24"/>
-      <c r="B22" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s" s="26">
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" ht="23" customHeight="1">
+      <c r="A22" s="23"/>
+      <c r="B22" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s" s="25">
         <v>50</v>
       </c>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23" ht="23" customHeight="1">
+      <c r="A23" s="23"/>
+      <c r="B23" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s" s="25">
+        <v>51</v>
+      </c>
+      <c r="D23" s="22"/>
+    </row>
+    <row r="24" ht="23" customHeight="1">
+      <c r="A24" t="s" s="20">
+        <v>52</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+    </row>
+    <row r="25" ht="23" customHeight="1">
+      <c r="A25" s="23"/>
+      <c r="B25" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s" s="25">
+        <v>53</v>
+      </c>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" ht="23" customHeight="1">
+      <c r="A26" s="23"/>
+      <c r="B26" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s" s="25">
+        <v>54</v>
+      </c>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27" ht="32" customHeight="1">
+      <c r="A27" s="23"/>
+      <c r="B27" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s" s="25">
+        <v>55</v>
+      </c>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" ht="32" customHeight="1">
+      <c r="A28" s="23"/>
+      <c r="B28" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s" s="25">
+        <v>56</v>
+      </c>
+      <c r="D28" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -4158,424 +4284,449 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:C48"/>
+  <dimension ref="A2:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.08594" style="27" customWidth="1"/>
-    <col min="2" max="2" width="2.54688" style="27" customWidth="1"/>
-    <col min="3" max="3" width="99.25" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="16.3516" style="27" customWidth="1"/>
+    <col min="1" max="1" width="5.08594" style="26" customWidth="1"/>
+    <col min="2" max="2" width="2.54688" style="26" customWidth="1"/>
+    <col min="3" max="3" width="99.25" style="26" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" ht="23" customHeight="1">
-      <c r="A2" t="s" s="21">
+      <c r="A2" t="s" s="20">
         <v>6</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" ht="23" customHeight="1">
-      <c r="A3" s="24"/>
-      <c r="B3" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s" s="26">
-        <v>52</v>
+      <c r="A3" s="23"/>
+      <c r="B3" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s" s="25">
+        <v>58</v>
       </c>
     </row>
     <row r="4" ht="23" customHeight="1">
-      <c r="A4" s="24"/>
-      <c r="B4" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s" s="26">
-        <v>53</v>
+      <c r="A4" s="23"/>
+      <c r="B4" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s" s="25">
+        <v>59</v>
       </c>
     </row>
     <row r="5" ht="23" customHeight="1">
-      <c r="A5" s="24"/>
-      <c r="B5" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s" s="26">
+      <c r="A5" s="23"/>
+      <c r="B5" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" ht="23" customHeight="1">
+      <c r="A6" s="23"/>
+      <c r="B6" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" ht="23" customHeight="1">
+      <c r="A7" t="s" s="20">
+        <v>8</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" ht="23" customHeight="1">
+      <c r="A8" s="23"/>
+      <c r="B8" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" ht="34" customHeight="1">
+      <c r="A9" s="23"/>
+      <c r="B9" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" ht="23" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" ht="23" customHeight="1">
+      <c r="A11" t="s" s="20">
+        <v>10</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+    </row>
+    <row r="12" ht="23" customHeight="1">
+      <c r="A12" s="23"/>
+      <c r="B12" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s" s="25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" ht="23" customHeight="1">
+      <c r="A13" s="23"/>
+      <c r="B13" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s" s="25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" ht="23" customHeight="1">
+      <c r="A14" s="23"/>
+      <c r="B14" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s" s="25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" ht="23" customHeight="1">
+      <c r="A15" s="23"/>
+      <c r="B15" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s" s="25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" ht="23" customHeight="1">
+      <c r="A16" s="23"/>
+      <c r="B16" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s" s="25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" ht="23" customHeight="1">
+      <c r="A17" t="s" s="20">
+        <v>70</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" ht="23" customHeight="1">
+      <c r="A18" s="23"/>
+      <c r="B18" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s" s="25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" ht="23" customHeight="1">
+      <c r="A19" t="s" s="20">
+        <v>13</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+    </row>
+    <row r="20" ht="23" customHeight="1">
+      <c r="A20" s="23"/>
+      <c r="B20" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s" s="25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" ht="23" customHeight="1">
+      <c r="A21" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+    </row>
+    <row r="22" ht="23" customHeight="1">
+      <c r="A22" s="23"/>
+      <c r="B22" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s" s="25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" ht="23" customHeight="1">
+      <c r="A23" s="23"/>
+      <c r="B23" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s" s="25">
         <v>54</v>
       </c>
     </row>
-    <row r="6" ht="23" customHeight="1">
-      <c r="A6" t="s" s="21">
-        <v>8</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-    </row>
-    <row r="7" ht="23" customHeight="1">
-      <c r="A7" s="24"/>
-      <c r="B7" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s" s="26">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" ht="32" customHeight="1">
-      <c r="A8" s="24"/>
-      <c r="B8" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s" s="26">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" ht="32" customHeight="1">
-      <c r="A9" s="24"/>
-      <c r="B9" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s" s="26">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" ht="23" customHeight="1">
-      <c r="A10" s="24"/>
-      <c r="B10" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s" s="26">
+    <row r="24" ht="32" customHeight="1">
+      <c r="A24" s="23"/>
+      <c r="B24" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s" s="25">
         <v>56</v>
       </c>
     </row>
-    <row r="11" ht="23" customHeight="1">
-      <c r="A11" t="s" s="21">
-        <v>10</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-    </row>
-    <row r="12" ht="23" customHeight="1">
-      <c r="A12" s="24"/>
-      <c r="B12" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s" s="26">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" ht="23" customHeight="1">
-      <c r="A13" s="24"/>
-      <c r="B13" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s" s="26">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" ht="23" customHeight="1">
-      <c r="A14" s="24"/>
-      <c r="B14" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s" s="26">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" ht="23" customHeight="1">
-      <c r="A15" s="24"/>
-      <c r="B15" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s" s="26">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" ht="23" customHeight="1">
-      <c r="A16" t="s" s="21">
-        <v>11</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-    </row>
-    <row r="17" ht="23" customHeight="1">
-      <c r="A17" s="24"/>
-      <c r="B17" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s" s="26">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" ht="23" customHeight="1">
-      <c r="A18" s="24"/>
-      <c r="B18" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s" s="26">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" ht="32" customHeight="1">
-      <c r="A19" s="24"/>
-      <c r="B19" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s" s="26">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" ht="32" customHeight="1">
-      <c r="A20" s="24"/>
-      <c r="B20" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C20" t="s" s="26">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" ht="23" customHeight="1">
-      <c r="A21" t="s" s="21">
+    <row r="25" ht="32" customHeight="1">
+      <c r="A25" s="23"/>
+      <c r="B25" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s" s="25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" ht="23" customHeight="1">
+      <c r="A26" t="s" s="20">
         <v>12</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-    </row>
-    <row r="22" ht="23" customHeight="1">
-      <c r="A22" s="24"/>
-      <c r="B22" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s" s="26">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" ht="23" customHeight="1">
-      <c r="A23" s="24"/>
-      <c r="B23" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s" s="26">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" ht="33" customHeight="1">
-      <c r="A24" s="24"/>
-      <c r="B24" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C24" t="s" s="26">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" ht="23" customHeight="1">
-      <c r="A25" t="s" s="21">
-        <v>13</v>
-      </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
-    </row>
-    <row r="26" ht="23" customHeight="1">
-      <c r="A26" s="24"/>
-      <c r="B26" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C26" t="s" s="26">
-        <v>66</v>
-      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
     </row>
     <row r="27" ht="23" customHeight="1">
-      <c r="A27" t="s" s="21">
+      <c r="A27" s="23"/>
+      <c r="B27" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s" s="25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" ht="23" customHeight="1">
+      <c r="A28" s="23"/>
+      <c r="B28" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s" s="25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" ht="33" customHeight="1">
+      <c r="A29" s="23"/>
+      <c r="B29" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s" s="25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" ht="23" customHeight="1">
+      <c r="A30" t="s" s="20">
         <v>14</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="23"/>
-    </row>
-    <row r="28" ht="23" customHeight="1">
-      <c r="A28" s="24"/>
-      <c r="B28" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C28" t="s" s="26">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" ht="32" customHeight="1">
-      <c r="A29" s="24"/>
-      <c r="B29" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s" s="26">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" ht="57" customHeight="1">
-      <c r="A30" s="24"/>
-      <c r="B30" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C30" t="s" s="26">
-        <v>69</v>
-      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
     </row>
     <row r="31" ht="23" customHeight="1">
-      <c r="A31" t="s" s="21">
+      <c r="A31" s="23"/>
+      <c r="B31" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s" s="25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" ht="32" customHeight="1">
+      <c r="A32" s="23"/>
+      <c r="B32" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s" s="25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" ht="57" customHeight="1">
+      <c r="A33" s="23"/>
+      <c r="B33" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" ht="23" customHeight="1">
+      <c r="A34" t="s" s="20">
         <v>15</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-    </row>
-    <row r="32" ht="23" customHeight="1">
-      <c r="A32" s="24"/>
-      <c r="B32" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s" s="26">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" ht="23" customHeight="1">
-      <c r="A33" s="24"/>
-      <c r="B33" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C33" t="s" s="26">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" ht="23" customHeight="1">
-      <c r="A34" s="24"/>
-      <c r="B34" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C34" t="s" s="26">
-        <v>72</v>
-      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
     </row>
     <row r="35" ht="23" customHeight="1">
-      <c r="A35" t="s" s="21">
+      <c r="A35" s="23"/>
+      <c r="B35" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s" s="25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" ht="23" customHeight="1">
+      <c r="A36" s="23"/>
+      <c r="B36" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s" s="25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" ht="23" customHeight="1">
+      <c r="A37" s="23"/>
+      <c r="B37" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s" s="25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" ht="23" customHeight="1">
+      <c r="A38" t="s" s="20">
         <v>16</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
-    </row>
-    <row r="36" ht="23" customHeight="1">
-      <c r="A36" s="24"/>
-      <c r="B36" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C36" t="s" s="26">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" ht="23" customHeight="1">
-      <c r="A37" s="24"/>
-      <c r="B37" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C37" t="s" s="26">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" ht="23" customHeight="1">
-      <c r="A38" s="24"/>
-      <c r="B38" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C38" t="s" s="26">
-        <v>75</v>
-      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="22"/>
     </row>
     <row r="39" ht="23" customHeight="1">
-      <c r="A39" t="s" s="21">
+      <c r="A39" s="23"/>
+      <c r="B39" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s" s="25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" ht="23" customHeight="1">
+      <c r="A40" s="23"/>
+      <c r="B40" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s" s="25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" ht="23" customHeight="1">
+      <c r="A41" s="23"/>
+      <c r="B41" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C41" t="s" s="25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" ht="23" customHeight="1">
+      <c r="A42" t="s" s="20">
         <v>17</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
-    </row>
-    <row r="40" ht="23" customHeight="1">
-      <c r="A40" s="24"/>
-      <c r="B40" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C40" t="s" s="26">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" ht="32" customHeight="1">
-      <c r="A41" s="24"/>
-      <c r="B41" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C41" t="s" s="26">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" ht="23" customHeight="1">
-      <c r="A42" s="24"/>
-      <c r="B42" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C42" t="s" s="26">
-        <v>78</v>
-      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
     </row>
     <row r="43" ht="23" customHeight="1">
-      <c r="A43" t="s" s="21">
+      <c r="A43" s="23"/>
+      <c r="B43" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C43" t="s" s="25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" ht="32" customHeight="1">
+      <c r="A44" s="23"/>
+      <c r="B44" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s" s="25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" ht="23" customHeight="1">
+      <c r="A45" s="23"/>
+      <c r="B45" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s" s="25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" ht="23" customHeight="1">
+      <c r="A46" t="s" s="20">
         <v>19</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="23"/>
-    </row>
-    <row r="44" ht="23" customHeight="1">
-      <c r="A44" s="24"/>
-      <c r="B44" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C44" t="s" s="26">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" ht="44" customHeight="1">
-      <c r="A45" s="24"/>
-      <c r="B45" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C45" t="s" s="26">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" ht="59" customHeight="1">
-      <c r="A46" s="24"/>
-      <c r="B46" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C46" t="s" s="26">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" ht="71" customHeight="1">
-      <c r="A47" s="24"/>
-      <c r="B47" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C47" t="s" s="26">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" ht="32" customHeight="1">
-      <c r="A48" s="24"/>
-      <c r="B48" t="s" s="25">
-        <v>31</v>
-      </c>
-      <c r="C48" t="s" s="26">
-        <v>83</v>
+      <c r="B46" s="21"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" ht="23" customHeight="1">
+      <c r="A47" s="23"/>
+      <c r="B47" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s" s="25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" ht="44" customHeight="1">
+      <c r="A48" s="23"/>
+      <c r="B48" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s" s="25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" ht="59" customHeight="1">
+      <c r="A49" s="23"/>
+      <c r="B49" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s" s="25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" ht="71" customHeight="1">
+      <c r="A50" s="23"/>
+      <c r="B50" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C50" t="s" s="25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" ht="32" customHeight="1">
+      <c r="A51" s="23"/>
+      <c r="B51" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C51" t="s" s="25">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add pass through sequencer type
</commit_message>
<xml_diff>
--- a/doc/elara-app-types.xlsx
+++ b/doc/elara-app-types.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="97">
   <si>
     <t>Elara Application Types (Overview)</t>
   </si>
@@ -365,6 +365,28 @@
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t xml:space="preserve"> that directly invokes command processor with sequenced commands; no command store is present</t>
+    </r>
+  </si>
+  <si>
+    <t>SequencerPassthroughApp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="1"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>SequencerProcessorApp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> that directly invokes a standard passthrough processor with every sequenced command;  the passthrough processor routes a single event for every command with the same payload as the command</t>
     </r>
   </si>
   <si>
@@ -4284,7 +4306,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:C51"/>
+  <dimension ref="A2:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -4466,73 +4488,71 @@
     </row>
     <row r="21" ht="23" customHeight="1">
       <c r="A21" t="s" s="20">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
     </row>
-    <row r="22" ht="23" customHeight="1">
+    <row r="22" ht="33" customHeight="1">
       <c r="A22" s="23"/>
       <c r="B22" t="s" s="24">
         <v>31</v>
       </c>
       <c r="C22" t="s" s="25">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" ht="23" customHeight="1">
-      <c r="A23" s="23"/>
-      <c r="B23" t="s" s="24">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s" s="25">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" ht="32" customHeight="1">
+      <c r="A23" t="s" s="20">
+        <v>11</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+    </row>
+    <row r="24" ht="23" customHeight="1">
       <c r="A24" s="23"/>
       <c r="B24" t="s" s="24">
         <v>31</v>
       </c>
       <c r="C24" t="s" s="25">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" ht="32" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" ht="23" customHeight="1">
       <c r="A25" s="23"/>
       <c r="B25" t="s" s="24">
         <v>31</v>
       </c>
       <c r="C25" t="s" s="25">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" ht="23" customHeight="1">
-      <c r="A26" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
-    </row>
-    <row r="27" ht="23" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" ht="32" customHeight="1">
+      <c r="A26" s="23"/>
+      <c r="B26" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s" s="25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" ht="32" customHeight="1">
       <c r="A27" s="23"/>
       <c r="B27" t="s" s="24">
         <v>31</v>
       </c>
       <c r="C27" t="s" s="25">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" ht="23" customHeight="1">
-      <c r="A28" s="23"/>
-      <c r="B28" t="s" s="24">
-        <v>31</v>
-      </c>
-      <c r="C28" t="s" s="25">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" ht="33" customHeight="1">
+      <c r="A28" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+    </row>
+    <row r="29" ht="23" customHeight="1">
       <c r="A29" s="23"/>
       <c r="B29" t="s" s="24">
         <v>31</v>
@@ -4542,31 +4562,31 @@
       </c>
     </row>
     <row r="30" ht="23" customHeight="1">
-      <c r="A30" t="s" s="20">
-        <v>14</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-    </row>
-    <row r="31" ht="23" customHeight="1">
+      <c r="A30" s="23"/>
+      <c r="B30" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s" s="25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" ht="33" customHeight="1">
       <c r="A31" s="23"/>
       <c r="B31" t="s" s="24">
         <v>31</v>
       </c>
       <c r="C31" t="s" s="25">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" ht="32" customHeight="1">
-      <c r="A32" s="23"/>
-      <c r="B32" t="s" s="24">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s" s="25">
         <v>79</v>
       </c>
     </row>
-    <row r="33" ht="57" customHeight="1">
+    <row r="32" ht="23" customHeight="1">
+      <c r="A32" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
+    </row>
+    <row r="33" ht="23" customHeight="1">
       <c r="A33" s="23"/>
       <c r="B33" t="s" s="24">
         <v>31</v>
@@ -4575,30 +4595,30 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" ht="23" customHeight="1">
-      <c r="A34" t="s" s="20">
-        <v>15</v>
-      </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-    </row>
-    <row r="35" ht="23" customHeight="1">
+    <row r="34" ht="32" customHeight="1">
+      <c r="A34" s="23"/>
+      <c r="B34" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s" s="25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" ht="57" customHeight="1">
       <c r="A35" s="23"/>
       <c r="B35" t="s" s="24">
         <v>31</v>
       </c>
       <c r="C35" t="s" s="25">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" ht="23" customHeight="1">
-      <c r="A36" s="23"/>
-      <c r="B36" t="s" s="24">
-        <v>31</v>
-      </c>
-      <c r="C36" t="s" s="25">
-        <v>82</v>
-      </c>
+      <c r="A36" t="s" s="20">
+        <v>15</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
     </row>
     <row r="37" ht="23" customHeight="1">
       <c r="A37" s="23"/>
@@ -4610,11 +4630,13 @@
       </c>
     </row>
     <row r="38" ht="23" customHeight="1">
-      <c r="A38" t="s" s="20">
-        <v>16</v>
-      </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22"/>
+      <c r="A38" s="23"/>
+      <c r="B38" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s" s="25">
+        <v>84</v>
+      </c>
     </row>
     <row r="39" ht="23" customHeight="1">
       <c r="A39" s="23"/>
@@ -4622,17 +4644,15 @@
         <v>31</v>
       </c>
       <c r="C39" t="s" s="25">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" ht="23" customHeight="1">
-      <c r="A40" s="23"/>
-      <c r="B40" t="s" s="24">
-        <v>31</v>
-      </c>
-      <c r="C40" t="s" s="25">
-        <v>85</v>
-      </c>
+      <c r="A40" t="s" s="20">
+        <v>16</v>
+      </c>
+      <c r="B40" s="21"/>
+      <c r="C40" s="22"/>
     </row>
     <row r="41" ht="23" customHeight="1">
       <c r="A41" s="23"/>
@@ -4644,11 +4664,13 @@
       </c>
     </row>
     <row r="42" ht="23" customHeight="1">
-      <c r="A42" t="s" s="20">
-        <v>17</v>
-      </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="22"/>
+      <c r="A42" s="23"/>
+      <c r="B42" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s" s="25">
+        <v>87</v>
+      </c>
     </row>
     <row r="43" ht="23" customHeight="1">
       <c r="A43" s="23"/>
@@ -4656,17 +4678,15 @@
         <v>31</v>
       </c>
       <c r="C43" t="s" s="25">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" ht="32" customHeight="1">
-      <c r="A44" s="23"/>
-      <c r="B44" t="s" s="24">
-        <v>31</v>
-      </c>
-      <c r="C44" t="s" s="25">
         <v>88</v>
       </c>
+    </row>
+    <row r="44" ht="23" customHeight="1">
+      <c r="A44" t="s" s="20">
+        <v>17</v>
+      </c>
+      <c r="B44" s="21"/>
+      <c r="C44" s="22"/>
     </row>
     <row r="45" ht="23" customHeight="1">
       <c r="A45" s="23"/>
@@ -4677,12 +4697,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" ht="23" customHeight="1">
-      <c r="A46" t="s" s="20">
-        <v>19</v>
-      </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="22"/>
+    <row r="46" ht="32" customHeight="1">
+      <c r="A46" s="23"/>
+      <c r="B46" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C46" t="s" s="25">
+        <v>90</v>
+      </c>
     </row>
     <row r="47" ht="23" customHeight="1">
       <c r="A47" s="23"/>
@@ -4690,19 +4712,17 @@
         <v>31</v>
       </c>
       <c r="C47" t="s" s="25">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" ht="44" customHeight="1">
-      <c r="A48" s="23"/>
-      <c r="B48" t="s" s="24">
-        <v>31</v>
-      </c>
-      <c r="C48" t="s" s="25">
         <v>91</v>
       </c>
     </row>
-    <row r="49" ht="59" customHeight="1">
+    <row r="48" ht="23" customHeight="1">
+      <c r="A48" t="s" s="20">
+        <v>19</v>
+      </c>
+      <c r="B48" s="21"/>
+      <c r="C48" s="22"/>
+    </row>
+    <row r="49" ht="23" customHeight="1">
       <c r="A49" s="23"/>
       <c r="B49" t="s" s="24">
         <v>31</v>
@@ -4711,7 +4731,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" ht="71" customHeight="1">
+    <row r="50" ht="44" customHeight="1">
       <c r="A50" s="23"/>
       <c r="B50" t="s" s="24">
         <v>31</v>
@@ -4720,13 +4740,31 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" ht="32" customHeight="1">
+    <row r="51" ht="59" customHeight="1">
       <c r="A51" s="23"/>
       <c r="B51" t="s" s="24">
         <v>31</v>
       </c>
       <c r="C51" t="s" s="25">
         <v>94</v>
+      </c>
+    </row>
+    <row r="52" ht="71" customHeight="1">
+      <c r="A52" s="23"/>
+      <c r="B52" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C52" t="s" s="25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" ht="32" customHeight="1">
+      <c r="A53" s="23"/>
+      <c r="B53" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="C53" t="s" s="25">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated diagram to reflect newest app names
</commit_message>
<xml_diff>
--- a/doc/elara-app-types.xlsx
+++ b/doc/elara-app-types.xlsx
@@ -368,7 +368,7 @@
     </r>
   </si>
   <si>
-    <t>SequencerPassthroughApp</t>
+    <t>PassthroughApp</t>
   </si>
   <si>
     <r>
@@ -378,7 +378,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>SequencerProcessorApp</t>
+      <t>ProcessorApp</t>
     </r>
     <r>
       <rPr>

</xml_diff>